<commit_message>
Update for final scores.
</commit_message>
<xml_diff>
--- a/NCAA-bracket-pool/2024/ncaa-results-m-2024.xlsx
+++ b/NCAA-bracket-pool/2024/ncaa-results-m-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\teds-code\NCAA-bracket-pool\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1430ED72-8819-49E4-9BE2-3BBABA419A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5DFCF8-E140-4067-B92B-26B93BE04ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8565" yWindow="3390" windowWidth="17025" windowHeight="15885" xr2:uid="{81BA0736-6BF6-4238-9C23-0D0B6D40DD40}"/>
+    <workbookView xWindow="29250" yWindow="180" windowWidth="21600" windowHeight="15630" xr2:uid="{81BA0736-6BF6-4238-9C23-0D0B6D40DD40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="137">
   <si>
     <t>E-R1-G1</t>
   </si>
@@ -269,9 +269,6 @@
     <t>FAU</t>
   </si>
   <si>
-    <t>San Diego St.</t>
-  </si>
-  <si>
     <t>UAB</t>
   </si>
   <si>
@@ -311,9 +308,6 @@
     <t>Grambling St.</t>
   </si>
   <si>
-    <t>Utah St.</t>
-  </si>
-  <si>
     <t>TCU</t>
   </si>
   <si>
@@ -447,6 +441,12 @@
   </si>
   <si>
     <t>Long Beach</t>
+  </si>
+  <si>
+    <t>San Diego St</t>
+  </si>
+  <si>
+    <t>Utah State</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,10 +888,10 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
         <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,10 +902,10 @@
         <v>67</v>
       </c>
       <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
         <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,10 +916,10 @@
         <v>67</v>
       </c>
       <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,10 +930,10 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
         <v>83</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,10 +944,10 @@
         <v>67</v>
       </c>
       <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
         <v>85</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,10 +958,10 @@
         <v>67</v>
       </c>
       <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,6 +971,12 @@
       <c r="B10" t="s">
         <v>68</v>
       </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -979,6 +985,12 @@
       <c r="B11" t="s">
         <v>68</v>
       </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -987,6 +999,12 @@
       <c r="B12" t="s">
         <v>68</v>
       </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -995,6 +1013,12 @@
       <c r="B13" t="s">
         <v>68</v>
       </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1003,6 +1027,12 @@
       <c r="B14" t="s">
         <v>69</v>
       </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1011,6 +1041,12 @@
       <c r="B15" t="s">
         <v>69</v>
       </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1019,6 +1055,12 @@
       <c r="B16" t="s">
         <v>70</v>
       </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1028,10 +1070,10 @@
         <v>67</v>
       </c>
       <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1042,10 +1084,10 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1056,10 +1098,10 @@
         <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,10 +1112,10 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,10 +1126,10 @@
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,10 +1140,10 @@
         <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,10 +1154,10 @@
         <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,10 +1168,10 @@
         <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,6 +1181,12 @@
       <c r="B25" t="s">
         <v>68</v>
       </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1147,6 +1195,12 @@
       <c r="B26" t="s">
         <v>68</v>
       </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1155,6 +1209,12 @@
       <c r="B27" t="s">
         <v>68</v>
       </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1163,6 +1223,12 @@
       <c r="B28" t="s">
         <v>68</v>
       </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1171,6 +1237,12 @@
       <c r="B29" t="s">
         <v>69</v>
       </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1179,6 +1251,12 @@
       <c r="B30" t="s">
         <v>69</v>
       </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1187,6 +1265,12 @@
       <c r="B31" t="s">
         <v>70</v>
       </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1196,10 +1280,10 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,10 +1294,10 @@
         <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,10 +1308,10 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,10 +1322,10 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,10 +1336,10 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,10 +1350,10 @@
         <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,10 +1364,10 @@
         <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,10 +1378,10 @@
         <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1307,6 +1391,12 @@
       <c r="B40" t="s">
         <v>68</v>
       </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1315,6 +1405,12 @@
       <c r="B41" t="s">
         <v>68</v>
       </c>
+      <c r="C41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1323,6 +1419,12 @@
       <c r="B42" t="s">
         <v>68</v>
       </c>
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1331,6 +1433,12 @@
       <c r="B43" t="s">
         <v>68</v>
       </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1339,6 +1447,12 @@
       <c r="B44" t="s">
         <v>69</v>
       </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1347,6 +1461,12 @@
       <c r="B45" t="s">
         <v>69</v>
       </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1355,6 +1475,12 @@
       <c r="B46" t="s">
         <v>70</v>
       </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1364,10 +1490,10 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,10 +1504,10 @@
         <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,10 +1518,10 @@
         <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,10 +1532,10 @@
         <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,10 +1546,10 @@
         <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,10 +1560,10 @@
         <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,10 +1574,10 @@
         <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,10 +1588,10 @@
         <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,6 +1601,12 @@
       <c r="B55" t="s">
         <v>68</v>
       </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1483,6 +1615,12 @@
       <c r="B56" t="s">
         <v>68</v>
       </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -1491,6 +1629,12 @@
       <c r="B57" t="s">
         <v>68</v>
       </c>
+      <c r="C57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -1499,6 +1643,12 @@
       <c r="B58" t="s">
         <v>68</v>
       </c>
+      <c r="C58" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1507,6 +1657,12 @@
       <c r="B59" t="s">
         <v>69</v>
       </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1515,6 +1671,12 @@
       <c r="B60" t="s">
         <v>69</v>
       </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1523,6 +1685,12 @@
       <c r="B61" t="s">
         <v>70</v>
       </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1531,6 +1699,12 @@
       <c r="B62" t="s">
         <v>71</v>
       </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -1539,6 +1713,12 @@
       <c r="B63" t="s">
         <v>71</v>
       </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -1546,6 +1726,12 @@
       </c>
       <c r="B64" t="s">
         <v>72</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>